<commit_message>
Works for all the prio roles
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -9,14 +9,14 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="18">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -24,316 +24,16 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri Light"/>
-      <family val="2"/>
-      <color theme="3"/>
-      <sz val="18"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <b val="1"/>
-      <color theme="3"/>
-      <sz val="15"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <b val="1"/>
-      <color theme="3"/>
-      <sz val="13"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <b val="1"/>
-      <color theme="3"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color rgb="FF006100"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color rgb="FF9C0006"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color rgb="FF9C5700"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color rgb="FF3F3F76"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <b val="1"/>
-      <color rgb="FF3F3F3F"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <b val="1"/>
-      <color rgb="FFFA7D00"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color rgb="FFFA7D00"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <b val="1"/>
-      <color theme="0"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color rgb="FFFF0000"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <i val="1"/>
-      <color rgb="FF7F7F7F"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color theme="0"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.7999816888943144"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.5999938962981048"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.3999755851924192"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.7999816888943144"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.5999938962981048"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.3999755851924192"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.7999816888943144"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.5999938962981048"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.3999755851924192"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.7999816888943144"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.5999938962981048"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.3999755851924192"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.7999816888943144"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.5999938962981048"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.3999755851924192"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.7999816888943144"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.5999938962981048"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.3999755851924192"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -341,157 +41,9 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.3999755851924192"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="42">
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9"/>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -499,49 +51,8 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Title" xfId="1" builtinId="15"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19"/>
-    <cellStyle name="Good" xfId="6" builtinId="26"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28"/>
-    <cellStyle name="Input" xfId="9" builtinId="20"/>
-    <cellStyle name="Output" xfId="10" builtinId="21"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="Note" xfId="15" builtinId="10"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53"/>
-    <cellStyle name="Total" xfId="17" builtinId="25"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -918,8 +429,8 @@
   </sheetPr>
   <dimension ref="A1:H180"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -997,11 +508,6 @@
       <c r="E2" t="n">
         <v>0</v>
       </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>RSROP</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -1071,11 +577,6 @@
       <c r="E5" t="n">
         <v>0</v>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>RSROP</t>
-        </is>
-      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -1765,11 +1266,16 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>RSROP</t>
         </is>
       </c>
       <c r="E35" t="n">
         <v>0</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>RSROP</t>
+        </is>
       </c>
     </row>
     <row r="36">
@@ -1926,16 +1432,11 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>RSROP</t>
+          <t>RSROP, RSRPS</t>
         </is>
       </c>
       <c r="E42" t="n">
         <v>0</v>
-      </c>
-      <c r="H42" t="inlineStr">
-        <is>
-          <t>RSROP</t>
-        </is>
       </c>
     </row>
     <row r="43">
@@ -2345,7 +1846,7 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>RSROP</t>
+          <t>RSROP, RSRPS</t>
         </is>
       </c>
       <c r="E60" t="n">
@@ -2353,7 +1854,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>RSROP</t>
+          <t>RSRPS</t>
         </is>
       </c>
     </row>
@@ -5018,11 +4519,16 @@
       </c>
       <c r="D176" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>RSRPS</t>
         </is>
       </c>
       <c r="E176" t="n">
         <v>0</v>
+      </c>
+      <c r="H176" t="inlineStr">
+        <is>
+          <t>RSRPS</t>
+        </is>
       </c>
     </row>
     <row r="177">

</xml_diff>